<commit_message>
Made chemtax comparison plots
</commit_message>
<xml_diff>
--- a/files/chem_compare.xlsx
+++ b/files/chem_compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Documents\R\calvert_spatial\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E2E3E2-06DB-4E02-A08F-DC33F035DC9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7A7519-56ED-4B55-A4F9-67CA901D2B2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14604" xr2:uid="{847E65ED-082E-4133-A6BA-05EE648D61E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D49318-05C0-4A39-BCDD-9B07F338D016}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1824,7 +1824,7 @@
         <v>10</v>
       </c>
       <c r="C37" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1">
         <v>9.1993446151415512E-2</v>
@@ -1862,7 +1862,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1">
         <v>2.4739981318513554E-2</v>
@@ -1900,7 +1900,7 @@
         <v>10</v>
       </c>
       <c r="C39" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1">
         <v>9.9466625601053238E-2</v>
@@ -1938,7 +1938,7 @@
         <v>10</v>
       </c>
       <c r="C40" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1">
         <v>0.34378309051195782</v>
@@ -1976,7 +1976,7 @@
         <v>10</v>
       </c>
       <c r="C41" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1">
         <v>5.45663641144832E-2</v>
@@ -2014,7 +2014,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1">
         <v>8.7330718330728505E-3</v>
@@ -2052,7 +2052,7 @@
         <v>10</v>
       </c>
       <c r="C43" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1">
         <v>1.6901839058846235E-2</v>
@@ -2090,7 +2090,7 @@
         <v>10</v>
       </c>
       <c r="C44" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1">
         <v>3.7572933360934258E-2</v>
@@ -2128,7 +2128,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1">
         <v>6.7892408619324371E-2</v>
@@ -2166,7 +2166,7 @@
         <v>10</v>
       </c>
       <c r="C46" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1">
         <v>2.4806501964728039E-2</v>
@@ -2204,7 +2204,7 @@
         <v>10</v>
       </c>
       <c r="C47" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1">
         <v>2.9496415518224239E-2</v>
@@ -2242,7 +2242,7 @@
         <v>10</v>
       </c>
       <c r="C48" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1">
         <v>9.0589672327041626E-3</v>
@@ -2280,7 +2280,7 @@
         <v>11</v>
       </c>
       <c r="C49" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49" s="1">
         <v>3.1949033650259175E-2</v>
@@ -2318,7 +2318,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1">
         <v>4.5337095235784851E-2</v>
@@ -2356,7 +2356,7 @@
         <v>11</v>
       </c>
       <c r="C51" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D51" s="1">
         <v>4.9798621485630669E-2</v>
@@ -2394,7 +2394,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" s="1">
         <v>0.12762610241770744</v>
@@ -2432,7 +2432,7 @@
         <v>11</v>
       </c>
       <c r="C53" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53" s="1">
         <v>0.15285706023375192</v>
@@ -2470,7 +2470,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" s="1">
         <v>4.5784567172328629E-2</v>
@@ -2508,7 +2508,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D55" s="1">
         <v>4.9809300940069079E-3</v>
@@ -2546,7 +2546,7 @@
         <v>11</v>
       </c>
       <c r="C56" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" s="1">
         <v>5.9647991632421814E-2</v>
@@ -2584,7 +2584,7 @@
         <v>11</v>
       </c>
       <c r="C57" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1">
         <v>0.13700295984745026</v>
@@ -2622,7 +2622,7 @@
         <v>11</v>
       </c>
       <c r="C58" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58" s="1">
         <v>4.581771045923233E-2</v>
@@ -2660,7 +2660,7 @@
         <v>11</v>
       </c>
       <c r="C59" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" s="1">
         <v>4.6027543644110359E-2</v>
@@ -2698,7 +2698,7 @@
         <v>11</v>
       </c>
       <c r="C60" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" s="1">
         <v>2.7345521065096062E-2</v>
@@ -2729,459 +2729,1751 @@
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>0</v>
+      <c r="A61" s="2">
+        <v>43598</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C61" s="1">
-        <v>2</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>9</v>
+      <c r="D61" s="1">
+        <v>0.34529886146386463</v>
+      </c>
+      <c r="E61" s="1">
+        <v>5.8517603126044071E-4</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0.26001383115847904</v>
+      </c>
+      <c r="G61" s="1">
+        <v>4.7043779050000012E-3</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0.32654663920402527</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <v>4.8354755563195795E-4</v>
+      </c>
+      <c r="L61" s="1">
+        <v>11.219763914744059</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
-        <v>43598</v>
+        <v>43625</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>0.34529886146386463</v>
+        <v>4.0146630257368088E-2</v>
       </c>
       <c r="E62" s="1">
-        <v>5.8517603126044071E-4</v>
+        <v>0.10461624463399251</v>
       </c>
       <c r="F62" s="1">
-        <v>0.26001383115847904</v>
+        <v>6.3052211577693626E-2</v>
       </c>
       <c r="G62" s="1">
-        <v>4.7043779050000012E-3</v>
+        <v>0.12366434435049693</v>
       </c>
       <c r="H62" s="1">
-        <v>0.32654663920402527</v>
+        <v>0.10689722249905269</v>
       </c>
       <c r="I62" s="1">
-        <v>0</v>
+        <v>0.17670399943987528</v>
       </c>
       <c r="J62" s="1">
-        <v>0</v>
+        <v>0.15212966501712799</v>
       </c>
       <c r="K62" s="1">
-        <v>4.8354755563195795E-4</v>
+        <v>0</v>
       </c>
       <c r="L62" s="1">
-        <v>11.219763914744059</v>
+        <v>2.0197590986887612</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
-        <v>43625</v>
+        <v>43653</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>4.0146630257368088E-2</v>
+        <v>9.2639637490113572E-2</v>
       </c>
       <c r="E63" s="1">
-        <v>0.10461624463399251</v>
+        <v>0.24132724851369858</v>
       </c>
       <c r="F63" s="1">
-        <v>6.3052211577693626E-2</v>
+        <v>0.20861587425072989</v>
       </c>
       <c r="G63" s="1">
-        <v>0.12366434435049693</v>
+        <v>9.5295251230709255E-4</v>
       </c>
       <c r="H63" s="1">
-        <v>0.10689722249905269</v>
+        <v>0.21828873952229819</v>
       </c>
       <c r="I63" s="1">
-        <v>0.17670399943987528</v>
+        <v>0.42808640499909717</v>
       </c>
       <c r="J63" s="1">
-        <v>0.15212966501712799</v>
+        <v>0.16103054334719977</v>
       </c>
       <c r="K63" s="1">
         <v>0</v>
       </c>
       <c r="L63" s="1">
-        <v>2.0197590986887612</v>
+        <v>3.4078625837961831</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>43653</v>
+        <v>43683</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>9.2639637490113572E-2</v>
+        <v>0.15141345312198004</v>
       </c>
       <c r="E64" s="1">
-        <v>0.24132724851369858</v>
+        <v>0.44289432466030121</v>
       </c>
       <c r="F64" s="1">
-        <v>0.20861587425072989</v>
+        <v>3.9932473873098694E-2</v>
       </c>
       <c r="G64" s="1">
-        <v>9.5295251230709255E-4</v>
+        <v>0.40476489563783008</v>
       </c>
       <c r="H64" s="1">
-        <v>0.21828873952229819</v>
+        <v>0.24675945192575455</v>
       </c>
       <c r="I64" s="1">
-        <v>0.42808640499909717</v>
+        <v>0.49629562596480054</v>
       </c>
       <c r="J64" s="1">
-        <v>0.16103054334719977</v>
+        <v>0.23891782263914743</v>
       </c>
       <c r="K64" s="1">
         <v>0</v>
       </c>
       <c r="L64" s="1">
-        <v>3.4078625837961831</v>
+        <v>3.1934294700622559</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>43683</v>
+        <v>43708</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C65" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65" s="1">
-        <v>0.15141345312198004</v>
+        <v>8.9671769489844635E-2</v>
       </c>
       <c r="E65" s="1">
-        <v>0.44289432466030121</v>
+        <v>0.42705908914407092</v>
       </c>
       <c r="F65" s="1">
-        <v>3.9932473873098694E-2</v>
+        <v>0.45890103777249652</v>
       </c>
       <c r="G65" s="1">
-        <v>0.40476489563783008</v>
+        <v>0.24979500720898309</v>
       </c>
       <c r="H65" s="1">
-        <v>0.24675945192575455</v>
+        <v>0.72672024369239807</v>
       </c>
       <c r="I65" s="1">
-        <v>0.49629562596480054</v>
+        <v>0.74909343322118127</v>
       </c>
       <c r="J65" s="1">
-        <v>0.23891782263914743</v>
+        <v>0.6942292948563894</v>
       </c>
       <c r="K65" s="1">
-        <v>0</v>
+        <v>0.97042649984359741</v>
       </c>
       <c r="L65" s="1">
-        <v>3.1934294700622559</v>
+        <v>0.46085867285728455</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>43708</v>
+        <v>43743</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C66" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66" s="1">
-        <v>8.9671769489844635E-2</v>
+        <v>4.7827934846282005E-2</v>
       </c>
       <c r="E66" s="1">
-        <v>0.42705908914407092</v>
+        <v>0.23116165151198706</v>
       </c>
       <c r="F66" s="1">
-        <v>0.45890103777249652</v>
+        <v>4.7194045657912888E-2</v>
       </c>
       <c r="G66" s="1">
-        <v>0.24979500720898309</v>
+        <v>0.12782647088170052</v>
       </c>
       <c r="H66" s="1">
-        <v>0.72672024369239807</v>
+        <v>0.21602871268987656</v>
       </c>
       <c r="I66" s="1">
-        <v>0.74909343322118127</v>
+        <v>0.18513061602910361</v>
       </c>
       <c r="J66" s="1">
-        <v>0.6942292948563894</v>
+        <v>0.17808936784664789</v>
       </c>
       <c r="K66" s="1">
-        <v>0.97042649984359741</v>
+        <v>0.39137032131354016</v>
       </c>
       <c r="L66" s="1">
-        <v>0.46085867285728455</v>
+        <v>0.50743784507115686</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <v>43743</v>
+        <v>43952</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1">
-        <v>4.7827934846282005E-2</v>
+        <v>0</v>
       </c>
       <c r="E67" s="1">
-        <v>0.23116165151198706</v>
+        <v>5.5383294845038711E-4</v>
       </c>
       <c r="F67" s="1">
-        <v>4.7194045657912888E-2</v>
+        <v>0.10900742436448733</v>
       </c>
       <c r="G67" s="1">
-        <v>0.12782647088170052</v>
+        <v>2.4121534952428192E-3</v>
       </c>
       <c r="H67" s="1">
-        <v>0.21602871268987656</v>
+        <v>9.8392597089211151E-2</v>
       </c>
       <c r="I67" s="1">
-        <v>0.18513061602910361</v>
+        <v>0.23444982369740805</v>
       </c>
       <c r="J67" s="1">
-        <v>0.17808936784664789</v>
+        <v>0</v>
       </c>
       <c r="K67" s="1">
-        <v>0.39137032131354016</v>
+        <v>0.26334954798221588</v>
       </c>
       <c r="L67" s="1">
-        <v>0.50743784507115686</v>
+        <v>4.3296091556549072</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
-        <v>43952</v>
+        <v>43990</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C68" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68" s="1">
-        <v>0</v>
+        <v>3.9948930963873863E-2</v>
       </c>
       <c r="E68" s="1">
-        <v>5.5383294845038711E-4</v>
+        <v>4.6537444616357483E-2</v>
       </c>
       <c r="F68" s="1">
-        <v>0.10900742436448733</v>
+        <v>9.1383475810289383E-2</v>
       </c>
       <c r="G68" s="1">
-        <v>2.4121534952428192E-3</v>
+        <v>0.11879933004577954</v>
       </c>
       <c r="H68" s="1">
-        <v>9.8392597089211151E-2</v>
+        <v>0.15001680453618368</v>
       </c>
       <c r="I68" s="1">
-        <v>0.23444982369740805</v>
+        <v>0.17695873975753784</v>
       </c>
       <c r="J68" s="1">
         <v>0</v>
       </c>
       <c r="K68" s="1">
-        <v>0.26334954798221588</v>
+        <v>9.3879625201225281E-2</v>
       </c>
       <c r="L68" s="1">
-        <v>4.3296091556549072</v>
+        <v>1.6485061446825664</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
-        <v>43990</v>
+        <v>44017</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" s="1">
-        <v>3.9948930963873863E-2</v>
+        <v>0.10727089395125707</v>
       </c>
       <c r="E69" s="1">
-        <v>4.6537444616357483E-2</v>
+        <v>6.050923160122087E-4</v>
       </c>
       <c r="F69" s="1">
-        <v>9.1383475810289383E-2</v>
+        <v>0.14373816549777985</v>
       </c>
       <c r="G69" s="1">
-        <v>0.11879933004577954</v>
+        <v>0.18190892537434897</v>
       </c>
       <c r="H69" s="1">
-        <v>0.15001680453618368</v>
+        <v>0.19996277242898941</v>
       </c>
       <c r="I69" s="1">
-        <v>0.17695873975753784</v>
+        <v>0.18252604951461157</v>
       </c>
       <c r="J69" s="1">
-        <v>0</v>
+        <v>0.10215928157170613</v>
       </c>
       <c r="K69" s="1">
-        <v>9.3879625201225281E-2</v>
+        <v>0.19011522581179938</v>
       </c>
       <c r="L69" s="1">
-        <v>1.6485061446825664</v>
+        <v>2.8803226153055825</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
-        <v>44017</v>
+        <v>44078</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70" s="1">
-        <v>0.10727089395125707</v>
+        <v>0.253380186855793</v>
       </c>
       <c r="E70" s="1">
-        <v>6.050923160122087E-4</v>
+        <v>0.23900587856769562</v>
       </c>
       <c r="F70" s="1">
-        <v>0.14373816549777985</v>
+        <v>0.16954833020766577</v>
       </c>
       <c r="G70" s="1">
-        <v>0.18190892537434897</v>
+        <v>0.35064138472080231</v>
       </c>
       <c r="H70" s="1">
-        <v>0.19996277242898941</v>
+        <v>0.31009345253308612</v>
       </c>
       <c r="I70" s="1">
-        <v>0.18252604951461157</v>
+        <v>0.17431948582331339</v>
       </c>
       <c r="J70" s="1">
-        <v>0.10215928157170613</v>
+        <v>0.31237075229485828</v>
       </c>
       <c r="K70" s="1">
-        <v>0.19011522581179938</v>
+        <v>0.36539415518442792</v>
       </c>
       <c r="L70" s="1">
-        <v>2.8803226153055825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
-        <v>44078</v>
+        <v>44106</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C71" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D71" s="1">
-        <v>0.253380186855793</v>
+        <v>2.6664969200889271E-2</v>
       </c>
       <c r="E71" s="1">
-        <v>0.23900587856769562</v>
+        <v>3.8414203872283302E-2</v>
       </c>
       <c r="F71" s="1">
-        <v>0.16954833020766577</v>
+        <v>3.3580514757583536E-2</v>
       </c>
       <c r="G71" s="1">
-        <v>0.35064138472080231</v>
+        <v>0.10134617115060489</v>
       </c>
       <c r="H71" s="1">
-        <v>0.31009345253308612</v>
+        <v>8.1602755934000015E-2</v>
       </c>
       <c r="I71" s="1">
-        <v>0.17431948582331339</v>
+        <v>0.12522100284695625</v>
       </c>
       <c r="J71" s="1">
-        <v>0.31237075229485828</v>
+        <v>0</v>
       </c>
       <c r="K71" s="1">
-        <v>0.36539415518442792</v>
+        <v>0.12006499742468198</v>
       </c>
       <c r="L71" s="1">
-        <v>0</v>
+        <v>0.28880057235558826</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
-        <v>44106</v>
+        <v>43599</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C72" s="1">
         <v>2</v>
       </c>
       <c r="D72" s="1">
-        <v>2.6664969200889271E-2</v>
+        <v>5.8079037194450699E-2</v>
       </c>
       <c r="E72" s="1">
-        <v>3.8414203872283302E-2</v>
+        <v>0.18680286655823389</v>
       </c>
       <c r="F72" s="1">
-        <v>3.3580514757583536E-2</v>
+        <v>0</v>
       </c>
       <c r="G72" s="1">
-        <v>0.10134617115060489</v>
+        <v>1.0933660864830017</v>
       </c>
       <c r="H72" s="1">
-        <v>8.1602755934000015E-2</v>
+        <v>1.2564922173817952</v>
       </c>
       <c r="I72" s="1">
-        <v>0.12522100284695625</v>
+        <v>0.28203985343376797</v>
       </c>
       <c r="J72" s="1">
-        <v>0</v>
+        <v>0.41156761844952899</v>
       </c>
       <c r="K72" s="1">
-        <v>0.12006499742468198</v>
+        <v>0</v>
       </c>
       <c r="L72" s="1">
-        <v>0.28880057235558826</v>
+        <v>2.7116385698318481</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>43627</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3.1395533432563148E-2</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1.9916105508552087E-3</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <v>4.5509558791915573E-2</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0.31397635241349536</v>
+      </c>
+      <c r="I73" s="1">
+        <v>4.6422836409571273E-3</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0</v>
+      </c>
+      <c r="K73" s="1">
+        <v>3.6244994650284448E-3</v>
+      </c>
+      <c r="L73" s="1">
+        <v>3.1561954021453857</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>43652</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="1">
+        <v>2</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.1042121301094691</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0.1253612165649732</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1">
+        <v>0.39757748941580456</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0.38732401033242542</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.39195378621419269</v>
+      </c>
+      <c r="J74" s="1">
+        <v>7.6839113608002663E-2</v>
+      </c>
+      <c r="K74" s="1">
+        <v>0</v>
+      </c>
+      <c r="L74" s="1">
+        <v>3.7819604078928628</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>43682</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="1">
+        <v>2</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.36812798182169598</v>
+      </c>
+      <c r="E75" s="1">
+        <v>9.5280889421701431E-2</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0.8679595788319906</v>
+      </c>
+      <c r="H75" s="1">
+        <v>1.4099781910578411</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0.22553920994202295</v>
+      </c>
+      <c r="J75" s="1">
+        <v>0.42207622528076172</v>
+      </c>
+      <c r="K75" s="1">
+        <v>0</v>
+      </c>
+      <c r="L75" s="1">
+        <v>0.75662921865781152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>43710</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="1">
+        <v>2</v>
+      </c>
+      <c r="D76" s="1">
+        <v>6.6009764249126121E-2</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1.6141078958753496E-3</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0.13912889113028845</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0.38025088111559552</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0.37930844227472943</v>
+      </c>
+      <c r="J76" s="1">
+        <v>9.7723590830961868E-2</v>
+      </c>
+      <c r="K76" s="1">
+        <v>4.3757260466615357E-2</v>
+      </c>
+      <c r="L76" s="1">
+        <v>5.8222202459971113</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>43742</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="1">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2.9421163722872734E-2</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0.55949842929840088</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0.27241930117209751</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0.16358589380979538</v>
+      </c>
+      <c r="J77" s="1">
+        <v>0.1702326163649559</v>
+      </c>
+      <c r="K77" s="1">
+        <v>4.4014479499310255E-4</v>
+      </c>
+      <c r="L77" s="1">
+        <v>0.35578807195027667</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>43955</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="1">
+        <v>2</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1.4465171378105879E-2</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1.8031590307752293E-2</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>9.4421836237112686E-2</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0.14810982843240103</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0.4534502426783244</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0.16121260076761246</v>
+      </c>
+      <c r="K78" s="1">
+        <v>0.31162555019060773</v>
+      </c>
+      <c r="L78" s="1">
+        <v>1.4824267824490864</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="1">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1">
+        <v>3.261924752344688E-2</v>
+      </c>
+      <c r="E79" s="1">
+        <v>4.8991493259867035E-2</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0.23057790348927179</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0.17922773708899817</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0.22664910306533179</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0.1740962490439415</v>
+      </c>
+      <c r="K79" s="1">
+        <v>0.25197609513998032</v>
+      </c>
+      <c r="L79" s="1">
+        <v>0.20520644386609396</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="1">
+        <v>2</v>
+      </c>
+      <c r="D80" s="1">
+        <v>6.8529004231095314E-2</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1.4500563944845149E-5</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0.22752143690983453</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0.19008940955003104</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0.10334217300017674</v>
+      </c>
+      <c r="J80" s="1">
+        <v>0.15809670959909758</v>
+      </c>
+      <c r="K80" s="1">
+        <v>0.18351355691750845</v>
+      </c>
+      <c r="L80" s="1">
+        <v>0.2612854813536008</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2</v>
+      </c>
+      <c r="D81" s="1">
+        <v>3.0442344956099987E-2</v>
+      </c>
+      <c r="E81" s="1">
+        <v>7.3435617741779424E-4</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>6.7855041474103928E-2</v>
+      </c>
+      <c r="H81" s="1">
+        <v>7.382241139809291E-2</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0.12496517846981685</v>
+      </c>
+      <c r="J81" s="1">
+        <v>0</v>
+      </c>
+      <c r="K81" s="1">
+        <v>0.27594951540231705</v>
+      </c>
+      <c r="L81" s="1">
+        <v>1.6158640185991924</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>44079</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="1">
+        <v>2</v>
+      </c>
+      <c r="D82" s="1">
+        <v>3.052957324932019E-2</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0.11183080946405728</v>
+      </c>
+      <c r="H82" s="1">
+        <v>7.8791312873363495E-2</v>
+      </c>
+      <c r="I82" s="1">
+        <v>6.2076253816485405E-2</v>
+      </c>
+      <c r="J82" s="1">
+        <v>0</v>
+      </c>
+      <c r="K82" s="1">
+        <v>0.11848556622862816</v>
+      </c>
+      <c r="L82" s="1">
+        <v>0.15576037019491196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>44108</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2</v>
+      </c>
+      <c r="D83" s="1">
+        <v>6.8375100381672382E-3</v>
+      </c>
+      <c r="E83" s="1">
+        <v>2.4437127945323784E-2</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0.12443226824204127</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0.10429592182238896</v>
+      </c>
+      <c r="I83" s="1">
+        <v>0.11113717903693517</v>
+      </c>
+      <c r="J83" s="1">
+        <v>8.1914203862349197E-2</v>
+      </c>
+      <c r="K83" s="1">
+        <v>0.13798153772950172</v>
+      </c>
+      <c r="L83" s="1">
+        <v>0.62115216255187988</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>43596</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="1">
+        <v>2</v>
+      </c>
+      <c r="D84" s="1">
+        <v>3.1491484493017197E-2</v>
+      </c>
+      <c r="E84" s="1">
+        <v>2.9649560029308002E-2</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0.31058841943740845</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0.56038232147693634</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0.4945816347996394</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0.11487464606761932</v>
+      </c>
+      <c r="K84" s="1">
+        <v>0</v>
+      </c>
+      <c r="L84" s="1">
+        <v>3.4336893955866494</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <v>43626</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="1">
+        <v>2</v>
+      </c>
+      <c r="D85" s="1">
+        <v>4.9335142907996975E-2</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0.19141835222641626</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0.32252218822638196</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0.30532543361186981</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0.29750298460324603</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0.12240575750668843</v>
+      </c>
+      <c r="K85" s="1">
+        <v>0</v>
+      </c>
+      <c r="L85" s="1">
+        <v>3.3803683121999106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
+        <v>43656</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="1">
+        <v>2</v>
+      </c>
+      <c r="D86" s="1">
+        <v>5.5904049426317215E-2</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0.10758755107720692</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>4.9568556249141693E-2</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0.10668858637412389</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0.28028812011082965</v>
+      </c>
+      <c r="J86" s="1">
+        <v>0.13504588976502419</v>
+      </c>
+      <c r="K86" s="1">
+        <v>0</v>
+      </c>
+      <c r="L86" s="1">
+        <v>0.86691261331240332</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <v>43680</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.14454475790262222</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0.17360866814851761</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0.25673606991767883</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0.298853799700737</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0.16023122270901999</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0.14874272545178732</v>
+      </c>
+      <c r="K87" s="1">
+        <v>0</v>
+      </c>
+      <c r="L87" s="1">
+        <v>0.43919627865155536</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <v>43709</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" s="1">
+        <v>2</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.16008835658431053</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0.29679504036903381</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0.61043584843476617</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0.72362034519513452</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0.56129248440265656</v>
+      </c>
+      <c r="J88" s="1">
+        <v>1.2586369415124257</v>
+      </c>
+      <c r="K88" s="1">
+        <v>0.30687763790289563</v>
+      </c>
+      <c r="L88" s="1">
+        <v>0.40687038004398346</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>43739</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="1">
+        <v>2</v>
+      </c>
+      <c r="D89" s="1">
+        <v>4.7965613504250847E-2</v>
+      </c>
+      <c r="E89" s="1">
+        <v>3.6767105882366501E-2</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0.16827849795420965</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0.13442556063334146</v>
+      </c>
+      <c r="I89" s="1">
+        <v>9.7938039650519684E-2</v>
+      </c>
+      <c r="J89" s="1">
+        <v>0.1930174802740415</v>
+      </c>
+      <c r="K89" s="1">
+        <v>0.13634876534342766</v>
+      </c>
+      <c r="L89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1.3986161444336176E-2</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1.750326540786773E-3</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0.13605550676584244</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0.17070487141609192</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0.38364636898040771</v>
+      </c>
+      <c r="J90" s="1">
+        <v>0</v>
+      </c>
+      <c r="K90" s="1">
+        <v>0.61567342281341553</v>
+      </c>
+      <c r="L90" s="1">
+        <v>7.9445663293202715</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A91" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2</v>
+      </c>
+      <c r="D91" s="1">
+        <v>6.7093317086497947E-2</v>
+      </c>
+      <c r="E91" s="1">
+        <v>0</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0.20489434401194254</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0.28588017076253891</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0.22334166864554086</v>
+      </c>
+      <c r="J91" s="1">
+        <v>0</v>
+      </c>
+      <c r="K91" s="1">
+        <v>0.22379689166943231</v>
+      </c>
+      <c r="L91" s="1">
+        <v>1.7618867953618367</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0.15871768196423849</v>
+      </c>
+      <c r="E92" s="1">
+        <v>3.5378782583090165E-3</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0.17028051366408667</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0.45871453483899433</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0.27488764127095539</v>
+      </c>
+      <c r="J92" s="1">
+        <v>0</v>
+      </c>
+      <c r="K92" s="1">
+        <v>2.0173866922656696E-2</v>
+      </c>
+      <c r="L92" s="1">
+        <v>4.6057407855987549</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2</v>
+      </c>
+      <c r="D93" s="1">
+        <v>5.206391836206118E-2</v>
+      </c>
+      <c r="E93" s="1">
+        <v>9.8585978150367737E-2</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1">
+        <v>6.2197398394346237E-2</v>
+      </c>
+      <c r="H93" s="1">
+        <v>0.16746682425340018</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0.19569060454765955</v>
+      </c>
+      <c r="J93" s="1">
+        <v>0.16048327336708704</v>
+      </c>
+      <c r="K93" s="1">
+        <v>0.31067969401677448</v>
+      </c>
+      <c r="L93" s="1">
+        <v>2.1526316006978354</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94" s="1">
+        <v>2</v>
+      </c>
+      <c r="D94" s="1">
+        <v>5.1077270259459816E-2</v>
+      </c>
+      <c r="E94" s="1">
+        <v>8.1985745579004288E-2</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0.25169923404852551</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0.20350925376017889</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0.14717932914694151</v>
+      </c>
+      <c r="J94" s="1">
+        <v>0</v>
+      </c>
+      <c r="K94" s="1">
+        <v>0.22047026952107748</v>
+      </c>
+      <c r="L94" s="1">
+        <v>0.56610461076100671</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2</v>
+      </c>
+      <c r="D95" s="1">
+        <v>2.8374935189882915E-2</v>
+      </c>
+      <c r="E95" s="1">
+        <v>6.3332810377081231E-2</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0.21187928567330042</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0.22424006462097168</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0.31986482938130695</v>
+      </c>
+      <c r="J95" s="1">
+        <v>0</v>
+      </c>
+      <c r="K95" s="1">
+        <v>0.22309314211209616</v>
+      </c>
+      <c r="L95" s="1">
+        <v>0.79415406783421838</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <v>43598</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0.4190932959318161</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0.10261288161079089</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0.42102934420108795</v>
+      </c>
+      <c r="I96" s="1">
+        <v>7.8523888987547252E-5</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0</v>
+      </c>
+      <c r="K96" s="1">
+        <v>9.6105478393534814E-3</v>
+      </c>
+      <c r="L96" s="1">
+        <v>11.204971790313721</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>43625</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" s="1">
+        <v>2</v>
+      </c>
+      <c r="D97" s="1">
+        <v>4.5757753774523735E-2</v>
+      </c>
+      <c r="E97" s="1">
+        <v>0.14376281450192133</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0.13794315109650293</v>
+      </c>
+      <c r="H97" s="1">
+        <v>0.14160432914892832</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0.19341975202163061</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0.10858304674426715</v>
+      </c>
+      <c r="K97" s="1">
+        <v>0</v>
+      </c>
+      <c r="L97" s="1">
+        <v>2.0158987045288086</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>43653</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0.1086512158314387</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0.33014175295829773</v>
+      </c>
+      <c r="F98" s="1">
+        <v>0</v>
+      </c>
+      <c r="G98" s="1">
+        <v>8.0207601810495063E-2</v>
+      </c>
+      <c r="H98" s="1">
+        <v>0.28763315081596375</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0.46921210984388989</v>
+      </c>
+      <c r="J98" s="1">
+        <v>0.13683901727199554</v>
+      </c>
+      <c r="K98" s="1">
+        <v>0</v>
+      </c>
+      <c r="L98" s="1">
+        <v>3.3461190462112427</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>43683</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0.17748161653677622</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.60496133069197333</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0.38275767862796783</v>
+      </c>
+      <c r="H99" s="1">
+        <v>0.32445302605628967</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0.5406431804100672</v>
+      </c>
+      <c r="J99" s="1">
+        <v>0.13935026278098425</v>
+      </c>
+      <c r="K99" s="1">
+        <v>0</v>
+      </c>
+      <c r="L99" s="1">
+        <v>3.0447603861490884</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>43708</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2</v>
+      </c>
+      <c r="D100" s="1">
+        <v>9.4812688107291862E-2</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.5813430746396383</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0.39566273490587872</v>
+      </c>
+      <c r="H100" s="1">
+        <v>0.95113041996955872</v>
+      </c>
+      <c r="I100" s="1">
+        <v>0.80831342935562134</v>
+      </c>
+      <c r="J100" s="1">
+        <v>0.63804347316424048</v>
+      </c>
+      <c r="K100" s="1">
+        <v>1.2169779539108276</v>
+      </c>
+      <c r="L100" s="1">
+        <v>0.14047139619166651</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>43743</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1">
+        <v>5.4925370961427689E-2</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0.31359513600667316</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0.13112878302733103</v>
+      </c>
+      <c r="H101" s="1">
+        <v>0.28152015308539075</v>
+      </c>
+      <c r="I101" s="1">
+        <v>0.19911518196264902</v>
+      </c>
+      <c r="J101" s="1">
+        <v>0.14585493629177412</v>
+      </c>
+      <c r="K101" s="1">
+        <v>0.48418139417966205</v>
+      </c>
+      <c r="L101" s="1">
+        <v>0.32174593706925708</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1.6817431896924973E-3</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0</v>
+      </c>
+      <c r="G102" s="1">
+        <v>4.2223587942620121E-2</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0.13765339429179826</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0.26019551604986191</v>
+      </c>
+      <c r="J102" s="1">
+        <v>0</v>
+      </c>
+      <c r="K102" s="1">
+        <v>0.35229249795277912</v>
+      </c>
+      <c r="L102" s="1">
+        <v>4.2437278429667158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2</v>
+      </c>
+      <c r="D103" s="1">
+        <v>4.6063357964158058E-2</v>
+      </c>
+      <c r="E103" s="1">
+        <v>6.5231233214338616E-2</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0.14213367799917856</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0.20398279776175818</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0.19491754720608392</v>
+      </c>
+      <c r="J103" s="1">
+        <v>0</v>
+      </c>
+      <c r="K103" s="1">
+        <v>0.12126569698254268</v>
+      </c>
+      <c r="L103" s="1">
+        <v>1.592436174551646</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
+        <v>44017</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" s="1">
+        <v>2</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0.12676616385579109</v>
+      </c>
+      <c r="E104" s="1">
+        <v>7.9398811309753603E-4</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0.22127541899681091</v>
+      </c>
+      <c r="H104" s="1">
+        <v>0.26823524634043378</v>
+      </c>
+      <c r="I104" s="1">
+        <v>0.20205769191185632</v>
+      </c>
+      <c r="J104" s="1">
+        <v>6.0814516618847847E-2</v>
+      </c>
+      <c r="K104" s="1">
+        <v>0.25175213068723679</v>
+      </c>
+      <c r="L104" s="1">
+        <v>2.8569138844807944</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0.29284293949604034</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0.31696311632792157</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0.37458844482898712</v>
+      </c>
+      <c r="H105" s="1">
+        <v>0.37526739637056988</v>
+      </c>
+      <c r="I105" s="1">
+        <v>0.17756351828575134</v>
+      </c>
+      <c r="J105" s="1">
+        <v>0.23607297986745834</v>
+      </c>
+      <c r="K105" s="1">
+        <v>0.40145528316497803</v>
+      </c>
+      <c r="L105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A106" s="2">
+        <v>44106</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" s="1">
+        <v>2</v>
+      </c>
+      <c r="D106" s="1">
+        <v>3.0853971838951111E-2</v>
+      </c>
+      <c r="E106" s="1">
+        <v>5.3338175018628441E-2</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0.10460902874668439</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0.10912452389796574</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0.13804074004292488</v>
+      </c>
+      <c r="J106" s="1">
+        <v>0</v>
+      </c>
+      <c r="K106" s="1">
+        <v>0.1557194764415423</v>
+      </c>
+      <c r="L106" s="1">
+        <v>0.22400920838117599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>